<commit_message>
repository python for excel
</commit_message>
<xml_diff>
--- a/xl/course_participants.xlsx
+++ b/xl/course_participants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/python-for-excel/material/ch04/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wilsonartllc207-my.sharepoint.com/personal/ddeolarte_ralphwilson_com_mx/Documents/Documents/GitHub/python-for-excel/xl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C3465C-E2E7-7547-83E7-56DB60E1F49F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{D4C3465C-E2E7-7547-83E7-56DB60E1F49F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5ED52EA0-53AF-42E1-A361-CE55B6665059}"/>
   <bookViews>
-    <workbookView xWindow="-3860" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{D8AE91DD-D984-C848-920F-CB3FB60A3001}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{D8AE91DD-D984-C848-920F-CB3FB60A3001}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -156,7 +156,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -456,12 +456,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="11.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -481,7 +481,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -501,7 +501,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1000</v>
       </c>
@@ -521,7 +521,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1002</v>
       </c>
@@ -541,7 +541,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1003</v>
       </c>

</xml_diff>